<commit_message>
Actividad completada. Se procede a evaluar programa principal con secuencia multifasta.
</commit_message>
<xml_diff>
--- a/resultados_stop_codons.xlsx
+++ b/resultados_stop_codons.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,15 +484,75 @@
           <t>Tiempo de cálculo 2</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Estimación 3</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Error relativo 3</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Tiempo de cálculo 3</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Estimación 4</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Error relativo 4</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Tiempo de cálculo 4</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Estimación 5</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Error relativo 5</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Tiempo de cálculo 5</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Estimación 6</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Error relativo 6</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Tiempo de cálculo 6</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Especie Desconocida</t>
+          <t>SalPENE enterica</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5223887952113582</v>
+        <v>0.5222259124651947</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -500,35 +560,71 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>31440</v>
+        <v>31098</v>
       </c>
       <c r="E2" t="n">
-        <v>77365.328125</v>
+        <v>75885.140625</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5882983454043296</v>
+        <v>1.440193601678565</v>
       </c>
       <c r="G2" t="n">
-        <v>3.337860107421875e-06</v>
+        <v>2.384185791015625e-06</v>
       </c>
       <c r="H2" t="n">
-        <v>19263.83396121379</v>
+        <v>72362.02278288326</v>
       </c>
       <c r="I2" t="n">
-        <v>0.8974869943952948</v>
+        <v>1.326902784194587</v>
       </c>
       <c r="J2" t="n">
-        <v>1.9073486328125e-06</v>
+        <v>3.576278686523438e-06</v>
+      </c>
+      <c r="K2" t="n">
+        <v>49196.07136530571</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.5819689808124545</v>
+      </c>
+      <c r="M2" t="n">
+        <v>2.384185791015625e-06</v>
+      </c>
+      <c r="N2" t="n">
+        <v>49196.07136530571</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.5819689808124545</v>
+      </c>
+      <c r="P2" t="n">
+        <v>9.5367431640625e-07</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>31098</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1.169843336256902e-16</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1.192092895507812e-06</v>
+      </c>
+      <c r="T2" t="n">
+        <v>31098</v>
+      </c>
+      <c r="U2" t="n">
+        <v>1.169843336256902e-16</v>
+      </c>
+      <c r="V2" t="n">
+        <v>7.152557373046875e-07</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Especie Desconocida</t>
+          <t>SalPENE enterica</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.5223887952113582</v>
+        <v>0.5222259124651947</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -536,35 +632,71 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>83236</v>
+        <v>81227</v>
       </c>
       <c r="E3" t="n">
-        <v>77365.328125</v>
+        <v>75885.140625</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5882983454043296</v>
+        <v>0.06576457797284155</v>
       </c>
       <c r="G3" t="n">
-        <v>3.337860107421875e-06</v>
+        <v>2.384185791015625e-06</v>
       </c>
       <c r="H3" t="n">
-        <v>19263.83396121379</v>
+        <v>72362.02278288326</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8974869943952948</v>
+        <v>0.1091383064389519</v>
       </c>
       <c r="J3" t="n">
-        <v>1.9073486328125e-06</v>
+        <v>1.668930053710938e-06</v>
+      </c>
+      <c r="K3" t="n">
+        <v>67965.39931341434</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.1632659175715669</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1.430511474609375e-06</v>
+      </c>
+      <c r="N3" t="n">
+        <v>67965.39931341434</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.1632659175715669</v>
+      </c>
+      <c r="P3" t="n">
+        <v>9.5367431640625e-07</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>81227</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>7.152557373046875e-07</v>
+      </c>
+      <c r="T3" t="n">
+        <v>81227</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>4.76837158203125e-07</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Especie Desconocida</t>
+          <t>SalPENE enterica</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5223887952113582</v>
+        <v>0.5222259124651947</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -572,25 +704,405 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>73240</v>
+        <v>72083</v>
       </c>
       <c r="E4" t="n">
-        <v>77365.328125</v>
+        <v>75885.140625</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5882983454043296</v>
+        <v>0.05274670345296394</v>
       </c>
       <c r="G4" t="n">
-        <v>3.337860107421875e-06</v>
+        <v>2.384185791015625e-06</v>
       </c>
       <c r="H4" t="n">
-        <v>19263.83396121379</v>
+        <v>66236.28128249325</v>
       </c>
       <c r="I4" t="n">
-        <v>0.8974869943952948</v>
+        <v>0.08111092376159083</v>
       </c>
       <c r="J4" t="n">
-        <v>1.9073486328125e-06</v>
+        <v>4.76837158203125e-07</v>
+      </c>
+      <c r="K4" t="n">
+        <v>67456.42165772074</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.06418404259366646</v>
+      </c>
+      <c r="M4" t="n">
+        <v>9.5367431640625e-07</v>
+      </c>
+      <c r="N4" t="n">
+        <v>67456.42165772074</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.06418404259366646</v>
+      </c>
+      <c r="P4" t="n">
+        <v>7.152557373046875e-07</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>72083</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>4.76837158203125e-07</v>
+      </c>
+      <c r="T4" t="n">
+        <v>72083</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="n">
+        <v>2.384185791015625e-07</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Salmonella enterica</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.5222259124651947</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>TAG</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>31098</v>
+      </c>
+      <c r="E5" t="n">
+        <v>75885.140625</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1.440193601678565</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2.86102294921875e-06</v>
+      </c>
+      <c r="H5" t="n">
+        <v>72362.02278288326</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1.326902784194587</v>
+      </c>
+      <c r="J5" t="n">
+        <v>2.145767211914062e-06</v>
+      </c>
+      <c r="K5" t="n">
+        <v>49196.07136530571</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.5819689808124545</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1.668930053710938e-06</v>
+      </c>
+      <c r="N5" t="n">
+        <v>49196.07136530571</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.5819689808124545</v>
+      </c>
+      <c r="P5" t="n">
+        <v>7.152557373046875e-07</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>31098</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1.169843336256902e-16</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1.192092895507812e-06</v>
+      </c>
+      <c r="T5" t="n">
+        <v>31098</v>
+      </c>
+      <c r="U5" t="n">
+        <v>1.169843336256902e-16</v>
+      </c>
+      <c r="V5" t="n">
+        <v>4.76837158203125e-07</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Salmonella enterica</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.5222259124651947</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>TGA</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>81227</v>
+      </c>
+      <c r="E6" t="n">
+        <v>75885.140625</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.06576457797284155</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2.86102294921875e-06</v>
+      </c>
+      <c r="H6" t="n">
+        <v>72362.02278288326</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.1091383064389519</v>
+      </c>
+      <c r="J6" t="n">
+        <v>7.152557373046875e-07</v>
+      </c>
+      <c r="K6" t="n">
+        <v>67965.39931341434</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.1632659175715669</v>
+      </c>
+      <c r="M6" t="n">
+        <v>4.76837158203125e-07</v>
+      </c>
+      <c r="N6" t="n">
+        <v>67965.39931341434</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.1632659175715669</v>
+      </c>
+      <c r="P6" t="n">
+        <v>4.76837158203125e-07</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>81227</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>7.152557373046875e-07</v>
+      </c>
+      <c r="T6" t="n">
+        <v>81227</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>2.384185791015625e-07</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Salmonella enterica</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.5222259124651947</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>TAA</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>72083</v>
+      </c>
+      <c r="E7" t="n">
+        <v>75885.140625</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.05274670345296394</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2.86102294921875e-06</v>
+      </c>
+      <c r="H7" t="n">
+        <v>66236.28128249325</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.08111092376159083</v>
+      </c>
+      <c r="J7" t="n">
+        <v>2.384185791015625e-07</v>
+      </c>
+      <c r="K7" t="n">
+        <v>67456.42165772074</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.06418404259366646</v>
+      </c>
+      <c r="M7" t="n">
+        <v>4.76837158203125e-07</v>
+      </c>
+      <c r="N7" t="n">
+        <v>67456.42165772074</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.06418404259366646</v>
+      </c>
+      <c r="P7" t="n">
+        <v>4.76837158203125e-07</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>72083</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>1.192092895507812e-06</v>
+      </c>
+      <c r="T7" t="n">
+        <v>72083</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V7" t="n">
+        <v>2.384185791015625e-07</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Promedios</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>75885.140625</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.5195682943681234</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2.622604370117188e-06</v>
+      </c>
+      <c r="H8" t="n">
+        <v>70320.10894941993</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.5057173381317098</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1.470247904459635e-06</v>
+      </c>
+      <c r="K8" t="n">
+        <v>61539.29744548027</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.2698063136592293</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1.231829325358073e-06</v>
+      </c>
+      <c r="N8" t="n">
+        <v>61539.29744548027</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.2698063136592293</v>
+      </c>
+      <c r="P8" t="n">
+        <v>7.152557373046875e-07</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>61469.33333333334</v>
+      </c>
+      <c r="R8" t="n">
+        <v>3.899477787523006e-17</v>
+      </c>
+      <c r="S8" t="n">
+        <v>9.139378865559896e-07</v>
+      </c>
+      <c r="T8" t="n">
+        <v>61469.33333333334</v>
+      </c>
+      <c r="U8" t="n">
+        <v>3.899477787523006e-17</v>
+      </c>
+      <c r="V8" t="n">
+        <v>3.973642985026042e-07</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Desviaciones estándar</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.7131370603801696</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2.611744678045111e-07</v>
+      </c>
+      <c r="H9" t="n">
+        <v>3163.319308557619</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.6362109940351867</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1.26534170532947e-06</v>
+      </c>
+      <c r="K9" t="n">
+        <v>9563.730950344632</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.2458266910820638</v>
+      </c>
+      <c r="M9" t="n">
+        <v>7.450977950626514e-07</v>
+      </c>
+      <c r="N9" t="n">
+        <v>9563.730950344632</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.2458266910820638</v>
+      </c>
+      <c r="P9" t="n">
+        <v>2.132480599880018e-07</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>23878.30145271365</v>
+      </c>
+      <c r="R9" t="n">
+        <v>6.041045011992937e-17</v>
+      </c>
+      <c r="S9" t="n">
+        <v>3.168964709818663e-07</v>
+      </c>
+      <c r="T9" t="n">
+        <v>23878.30145271365</v>
+      </c>
+      <c r="U9" t="n">
+        <v>6.041045011992937e-17</v>
+      </c>
+      <c r="V9" t="n">
+        <v>1.946679546660724e-07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>